<commit_message>
Test, but not successful
</commit_message>
<xml_diff>
--- a/notch_files/histogram.xlsx
+++ b/notch_files/histogram.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="75" windowWidth="11475" windowHeight="6735" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="75" windowWidth="11475" windowHeight="6735" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet7" sheetId="7" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
   <si>
     <t>a</t>
   </si>
@@ -42,9 +41,6 @@
     <t>bits required</t>
   </si>
   <si>
-    <t>x*y</t>
-  </si>
-  <si>
     <t>x (input interval)</t>
   </si>
   <si>
@@ -76,6 +72,12 @@
   </si>
   <si>
     <t xml:space="preserve"> bits signed</t>
+  </si>
+  <si>
+    <t>unscaled (x*ab - x*y)</t>
+  </si>
+  <si>
+    <t>y*ab</t>
   </si>
 </sst>
 </file>
@@ -117,27 +119,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="9">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -525,10 +507,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B34" sqref="B33:B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,7 +523,7 @@
     <col min="6" max="6" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -549,139 +531,161 @@
         <v>1</v>
       </c>
       <c r="C1">
-        <v>-3.9538619186602002</v>
+        <v>-1.9762267517966601</v>
       </c>
       <c r="D1">
-        <v>5.9025952860868296</v>
+        <v>0.99712125134943197</v>
       </c>
       <c r="E1">
-        <v>-3.9426719507494998</v>
+        <v>-1</v>
       </c>
       <c r="F1">
-        <v>0.99434776735846897</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-1.9776292392088199</v>
+      </c>
+      <c r="G1">
+        <v>0.99721251792941201</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>0.88872562467175198</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>-3.51889660955815</v>
+        <v>-1.97974040218004</v>
       </c>
       <c r="D2">
-        <v>5.2607066554283897</v>
+        <v>1</v>
       </c>
       <c r="E2">
-        <v>-3.51889660955815</v>
+        <v>1</v>
       </c>
       <c r="F2">
-        <v>0.88872562467175198</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-1.97974556361571</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4">
         <f>TRUNC(B1*B10)</f>
-        <v>5461</v>
+        <v>16383</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:F4" si="0">TRUNC(C1*C10)</f>
-        <v>-21592</v>
+        <v>-32376</v>
       </c>
       <c r="D4">
         <f t="shared" si="0"/>
-        <v>32234</v>
+        <v>16335</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>-21530</v>
+        <v>-16383</v>
       </c>
       <c r="F4">
         <f t="shared" si="0"/>
-        <v>5430</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>-32399</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4" si="1">TRUNC(G1*G10)</f>
+        <v>16337</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <f>ABS( (B4/B10) - B1 )</f>
         <v>0</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:D5" si="1">ABS( (C4/C10) - C1 )</f>
-        <v>7.3132765709971181E-6</v>
+        <f t="shared" ref="C5:D5" si="2">ABS( (C4/C10) - C1 )</f>
+        <v>3.1915686057537584E-5</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>1.33413880565314E-5</v>
+        <f t="shared" si="2"/>
+        <v>5.1117674280898306E-5</v>
       </c>
       <c r="E5">
         <f>ABS( (E4/E10) - E1 )</f>
-        <v>1.7057737465986378E-4</v>
+        <v>0</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5" si="2">ABS( (F4/F10) - F1 )</f>
-        <v>2.4383362863811264E-5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F5:G5" si="3">ABS( (F4/F10) - F1 )</f>
+        <v>3.0508817560725987E-5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="3"/>
+        <v>2.030649072559676E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <f>TRUNC(B2*B10)</f>
-        <v>4853</v>
+        <v>16383</v>
       </c>
       <c r="C6">
-        <f t="shared" ref="C6:D6" si="3">TRUNC(C2*C10)</f>
-        <v>-19216</v>
+        <f t="shared" ref="C6:D6" si="4">TRUNC(C2*C10)</f>
+        <v>-32434</v>
       </c>
       <c r="D6">
-        <f t="shared" si="3"/>
-        <v>28728</v>
+        <f t="shared" si="4"/>
+        <v>16383</v>
       </c>
       <c r="E6">
         <f>TRUNC(E2*E10)</f>
-        <v>-19216</v>
+        <v>16383</v>
       </c>
       <c r="F6">
-        <f t="shared" ref="F6" si="4">TRUNC(F2*F10)</f>
-        <v>4853</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F6:G6" si="5">TRUNC(F2*F10)</f>
+        <v>-32434</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="5"/>
+        <v>16383</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <f>ABS( (B6/B10) - B2 )</f>
-        <v>6.0545016011270825E-5</v>
+        <v>0</v>
       </c>
       <c r="C7">
-        <f t="shared" ref="C7:D7" si="5">ABS( (C6/C10) - C2 )</f>
-        <v>1.2715341458635621E-4</v>
+        <f t="shared" ref="C7:D7" si="6">ABS( (C6/C10) - C2 )</f>
+        <v>5.3109269118056801E-6</v>
       </c>
       <c r="D7">
-        <f t="shared" si="5"/>
-        <v>1.3166916213780411E-4</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
       <c r="E7">
         <f>ABS( (E6/E10) - E2 )</f>
-        <v>1.2715341458635621E-4</v>
+        <v>0</v>
       </c>
       <c r="F7">
-        <f t="shared" ref="F7" si="6">ABS( (F6/F10) - F2 )</f>
-        <v>6.0545016011270825E-5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="F7:G7" si="7">ABS( (F6/F10) - F2 )</f>
+        <v>1.0472362581781525E-5</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -694,19 +698,23 @@
         <v>1</v>
       </c>
       <c r="D8" t="b">
-        <f t="shared" ref="D8:F8" si="7">(D4&lt;2^15-1)*D4&gt;(-2^15+1)</f>
+        <f t="shared" ref="D8:F8" si="8">(D4&lt;2^15-1)*D4&gt;(-2^15+1)</f>
         <v>1</v>
       </c>
       <c r="E8" t="b">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="F8" t="b">
-        <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="G8" t="b">
+        <f t="shared" ref="G8" si="9">(G4&lt;2^15-1)*G4&gt;(-2^15+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -715,45 +723,62 @@
         <v>1</v>
       </c>
       <c r="C9" t="b">
-        <f t="shared" ref="C9:F9" si="8">(C6&lt;2^15-1)*C6&gt;(-2^15+1)</f>
+        <f t="shared" ref="C9:F9" si="10">(C6&lt;2^15-1)*C6&gt;(-2^15+1)</f>
         <v>1</v>
       </c>
       <c r="D9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="E9" t="b">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="F9" t="b">
-        <f t="shared" si="8"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+      <c r="G9" t="b">
+        <f t="shared" ref="G9" si="11">(G6&lt;2^15-1)*G6&gt;(-2^15+1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10">
-        <v>5461</v>
+        <v>16383</v>
       </c>
       <c r="C10">
-        <v>5461</v>
+        <f>B10</f>
+        <v>16383</v>
       </c>
       <c r="D10">
-        <v>5461</v>
+        <f t="shared" ref="D10:G10" si="12">C10</f>
+        <v>16383</v>
       </c>
       <c r="E10">
-        <v>5461</v>
+        <f t="shared" si="12"/>
+        <v>16383</v>
       </c>
       <c r="F10">
-        <v>5461</v>
+        <f t="shared" si="12"/>
+        <v>16383</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="12"/>
+        <v>16383</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B8:F9">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G8:G9">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -763,10 +788,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +805,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1">
         <f>-2^(D1-1)+1</f>
@@ -794,25 +819,23 @@
         <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <f>MIN(Sheet2!B4:D6)</f>
-        <v>-21592</v>
+        <v>-32766</v>
       </c>
       <c r="C2">
-        <f>MAX(Sheet2!B4:D6)</f>
-        <v>32234</v>
+        <v>32766</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3">
         <f>-2^(D3-1)</f>
@@ -826,20 +849,20 @@
         <v>32</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <f>MIN(B1*B2,B1*C2,C1*B2,C1*C2)</f>
-        <v>-69221987877398</v>
+        <v>-70364449177602</v>
       </c>
       <c r="C5">
         <f>MAX(B1*B2,B1*C2,C1*B2,C1*C2)</f>
-        <v>69221987877398</v>
+        <v>70364449177602</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -848,11 +871,11 @@
       </c>
       <c r="B6">
         <f>LOG(-1*B5,2)+1</f>
-        <v>46.976295606123792</v>
+        <v>46.999911941523614</v>
       </c>
       <c r="C6">
         <f>LOG(C5,2)+1</f>
-        <v>46.976295606123792</v>
+        <v>46.999911941523614</v>
       </c>
       <c r="D6">
         <f>CEILING(MAX(B6:C6),1)</f>
@@ -861,23 +884,23 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9">
         <f>3*B5</f>
-        <v>-207665963632194</v>
+        <v>-211093347532806</v>
       </c>
       <c r="C9">
         <f>3*C5</f>
-        <v>207665963632194</v>
+        <v>211093347532806</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -886,11 +909,11 @@
       </c>
       <c r="B10">
         <f>LOG(-1*B9,2)+1</f>
-        <v>48.561258106844946</v>
+        <v>48.584874442244775</v>
       </c>
       <c r="C10">
         <f>LOG(C9,2)+1</f>
-        <v>48.561258106844946</v>
+        <v>48.584874442244775</v>
       </c>
       <c r="D10">
         <f>CEILING(MAX(B10:C10),1)</f>
@@ -899,15 +922,15 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B12">
-        <f>MIN(B1*B3,B1*C3,C1*B3,C1*C3)</f>
-        <v>-4.6116860162799043E+18</v>
+        <f>MIN(B2*B3,B2*C3,C2*B3,C2*C3)</f>
+        <v>-70364449210368</v>
       </c>
       <c r="C12">
-        <f>MAX(B1*B3,B1*C3,C1*B3,C1*C3)</f>
-        <v>4.6116860162799043E+18</v>
+        <f>MAX(B2*B3,B2*C3,C2*B3,C2*C3)</f>
+        <v>70364449210368</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -916,28 +939,28 @@
       </c>
       <c r="B13">
         <f>LOG(-1*B12,2)+1</f>
-        <v>62.999999999328196</v>
+        <v>46.999911942195425</v>
       </c>
       <c r="C13">
         <f>LOG(C12,2)+1</f>
-        <v>62.999999999328196</v>
+        <v>46.999911942195425</v>
       </c>
       <c r="D13">
         <f>CEILING(MAX(B13:C13),1)</f>
-        <v>63</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15">
         <f>B12*(B8-1)</f>
-        <v>-1.8446744065119617E+19</v>
+        <v>-140728898420736</v>
       </c>
       <c r="C15">
         <f>C12*(B8-1)</f>
-        <v>1.8446744065119617E+19</v>
+        <v>140728898420736</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -946,28 +969,28 @@
       </c>
       <c r="B16">
         <f>LOG(-1*B15,2)+1</f>
-        <v>64.999999999328196</v>
+        <v>47.999911942195425</v>
       </c>
       <c r="C16">
         <f>LOG(C15,2)+1</f>
-        <v>64.999999999328196</v>
+        <v>47.999911942195425</v>
       </c>
       <c r="D16">
         <f>CEILING(MAX(B16:C16),1)</f>
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <f>B5-C15</f>
-        <v>-1.8446813287107494E+19</v>
+        <v>-211093347598338</v>
       </c>
       <c r="C18">
         <f>C5-B15</f>
-        <v>1.8446813287107494E+19</v>
+        <v>211093347598338</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -976,61 +999,84 @@
       </c>
       <c r="B19">
         <f>LOG(-1*B18,2)+1</f>
-        <v>65.000005413076593</v>
+        <v>48.584874442692637</v>
       </c>
       <c r="C19">
         <f>LOG(C18,2)+1</f>
-        <v>65.000005413076593</v>
+        <v>48.584874442692637</v>
       </c>
       <c r="D19">
         <f>CEILING(MAX(B19:C19),1)</f>
-        <v>66</v>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f>B18/Sheet2!B10</f>
+        <v>-12884901886</v>
+      </c>
+      <c r="C21">
+        <f>C18/Sheet2!C10</f>
+        <v>12884901886</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B22">
+        <f>LOG(-1*B21,2)+1</f>
+        <v>34.58496250049722</v>
+      </c>
+      <c r="C22">
+        <f>LOG(C21,2)+1</f>
+        <v>34.58496250049722</v>
+      </c>
+      <c r="D22">
+        <f>CEILING(MAX(B22:C22),1)</f>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:D9 D17:D18 D11 D20:D1048576">
-    <cfRule type="cellIs" dxfId="10" priority="7" operator="greaterThan">
+  <conditionalFormatting sqref="D1:D9 D17:D18 D11 D20:D21 D23:D1048576">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D12:D14">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D10">
-    <cfRule type="cellIs" dxfId="8" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D15">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="greaterThan">
+      <formula>32</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
       <formula>32</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AFJ1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>